<commit_message>
MSE results of 80/20 5 fold cross validation added
- Results available in Excel spreadsheets as well as in notebook itself.
- ../_RESULTS/obj contains Python dictionaries with results of cross validation and mse calculation to be loaded without having to rerun these operations.
</commit_message>
<xml_diff>
--- a/_RESULTS/MSE_classic.xlsx
+++ b/_RESULTS/MSE_classic.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documenten\Programming\Python\Jupyter_Notebooks\PROJECTS\Compositional_data_kriging\_RESULTS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,8 +42,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,24 +95,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -145,9 +162,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,9 +196,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,9 +231,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,74 +407,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>32.09482503733238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
+      <c r="C2" s="3">
+        <v>32.094825037332377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>26.05522595007908</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>17.34698046573147</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>26.45209613756244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1"/>
+      <c r="C5" s="3">
+        <v>26.452096137562439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>10.777914304707</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>22.3386933672255</v>
+      <c r="C7" s="3">
+        <v>22.338693367225499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>